<commit_message>
inital commit for feature/symbol format refactoring
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/RefreshableResetOriginal_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/RefreshableResetOriginal_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gunxgar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>VERSION</t>
   </si>
@@ -186,6 +186,48 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>SYMBOL_2017</t>
+  </si>
+  <si>
+    <t>CIVIC NATURAL GAS</t>
+  </si>
+  <si>
+    <t>SED</t>
+  </si>
+  <si>
+    <t>1.8L L4 COMPRESSED NATURAL GAS</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>FRNT/HEAD/SIDE/REAR SIDE AIRBAGS</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>4 WHEEL STANDARD</t>
+  </si>
+  <si>
+    <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
+  </si>
+  <si>
+    <t>BI047</t>
+  </si>
+  <si>
+    <t>PD043</t>
+  </si>
+  <si>
+    <t>UM061</t>
+  </si>
+  <si>
+    <t>MP061</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -234,12 +276,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -521,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,8 +812,136 @@
         <v>38</v>
       </c>
     </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="2">
+        <v>26155</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2">
+        <v>2</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>51</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>60</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG3">
+        <v>20180319</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<WrappedLabelHistory xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2016/02/Classifier/internal/wrappedLabelHistory">
+  <Value>PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXMtYXNjaWkiPz48bGFiZWxIaXN0b3J5IHhtbG5zOnhzaT0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEtaW5zdGFuY2UiIHhtbG5zOnhzZD0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEiIHhtbG5zPSJodHRwOi8vd3d3LmJvbGRvbmphbWVzLmNvbS8yMDE2LzAyL0NsYXNzaWZpZXIvaW50ZXJuYWwvbGFiZWxIaXN0b3J5Ij48aXRlbT48c2lzbCBzaXNsVmVyc2lvbj0iMCIgcG9saWN5PSJhZDU3ZDYxOC03ZWI5LTQ4MzYtOTY1OS05MmUxYzk3ZDViMmIiIG9yaWdpbj0idXNlclNlbGVjdGVkIj48ZWxlbWVudCB1aWQ9IjBkZjlhOWJkLWZlYjEtNGIwMS05MjIyLTRlMWUzMWIxNDk4NCIgdmFsdWU9IiIgeG1sbnM9Imh0dHA6Ly93d3cuYm9sZG9uamFtZXMuY29tLzIwMDgvMDEvc2llL2ludGVybmFsL2xhYmVsIiAvPjwvc2lzbD48VXNlck5hbWU+RU5UXGd3M2VyYWo8L1VzZXJOYW1lPjxEYXRlVGltZT4xLzMxLzIwMTkgNDowNzowNSBQTTwvRGF0ZVRpbWU+PExhYmVsU3RyaW5nPkNvbmZpZGVudGlhbDwvTGFiZWxTdHJpbmc+PC9pdGVtPjwvbGFiZWxIaXN0b3J5Pg==</Value>
+</WrappedLabelHistory>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<sisl xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="ad57d618-7eb9-4836-9659-92e1c97d5b2b" origin="userSelected">
+  <element uid="0df9a9bd-feb1-4b01-9222-4e1e31b14984" value=""/>
+</sisl>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FCA150D-E8D2-4ACF-BD33-CC3838406F2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.boldonjames.com/2016/02/Classifier/internal/wrappedLabelHistory"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762F2E29-F018-496C-86EF-38B647DEFF82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>